<commit_message>
Final Final Delivery files
</commit_message>
<xml_diff>
--- a/Final Delivery/LabIACD_2324_GroupEvaluation_TP1_Group1.xlsx
+++ b/Final Delivery/LabIACD_2324_GroupEvaluation_TP1_Group1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EE87AB5-90BB-40A4-8DFF-15B0C1A54E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B740A71-D6B5-45E6-8B67-F97EA43BA826}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -79,9 +79,6 @@
     <t>-</t>
   </si>
   <si>
-    <t>Custom k-fold CV, "train-test-split" functions and PCA implementation; XGBoost parameters hypertunning; Model statistical analysis/comparison implementation; Video scripts, voice over and edition.</t>
-  </si>
-  <si>
     <t>PyRadiomics Features extraction; Random Forest and Neural Networks parameters hypertuning; Jupyter Notebooks assembly and markdown/comments; all code documentation; Video voice over.</t>
   </si>
   <si>
@@ -89,6 +86,9 @@
   </si>
   <si>
     <t>PyLidc features extraction; Data exploration, cleaning and transformation; Video visuals preparation, script and voice over.</t>
+  </si>
+  <si>
+    <t>Custom k-fold CV, "train-test-split" functions and PCA implementation; XGBoost parameters hypertuning; Model statistical analysis/comparison implementation; Video scripts, voice over and edition.</t>
   </si>
 </sst>
 </file>
@@ -458,7 +458,7 @@
   <dimension ref="D3:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -517,7 +517,7 @@
         <v>0.25</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>10</v>
@@ -531,7 +531,7 @@
         <v>0.25</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>10</v>
@@ -545,7 +545,7 @@
         <v>0.25</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>10</v>
@@ -559,7 +559,7 @@
         <v>0.25</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>10</v>

</xml_diff>